<commit_message>
After writing the second article
</commit_message>
<xml_diff>
--- a/Практическая часть/Входные данные/data.xlsx
+++ b/Практическая часть/Входные данные/data.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Магистратура\Диссертация\Практическая часть\Входные данные\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F61619-C06F-4C49-9E1D-F7918FDE3163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1205" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1325" uniqueCount="536">
   <si>
     <t>№</t>
   </si>
@@ -1505,13 +1510,139 @@
   </si>
   <si>
     <t>131;</t>
+  </si>
+  <si>
+    <t>241</t>
+  </si>
+  <si>
+    <t>242</t>
+  </si>
+  <si>
+    <t>243</t>
+  </si>
+  <si>
+    <t>244</t>
+  </si>
+  <si>
+    <t>245</t>
+  </si>
+  <si>
+    <t>246</t>
+  </si>
+  <si>
+    <t>247</t>
+  </si>
+  <si>
+    <t>248</t>
+  </si>
+  <si>
+    <t>249</t>
+  </si>
+  <si>
+    <t>250</t>
+  </si>
+  <si>
+    <t>251</t>
+  </si>
+  <si>
+    <t>252</t>
+  </si>
+  <si>
+    <t>253</t>
+  </si>
+  <si>
+    <t>254</t>
+  </si>
+  <si>
+    <t>255</t>
+  </si>
+  <si>
+    <t>256</t>
+  </si>
+  <si>
+    <t>257</t>
+  </si>
+  <si>
+    <t>258</t>
+  </si>
+  <si>
+    <t>259</t>
+  </si>
+  <si>
+    <t>260</t>
+  </si>
+  <si>
+    <t>261</t>
+  </si>
+  <si>
+    <t>262</t>
+  </si>
+  <si>
+    <t>263</t>
+  </si>
+  <si>
+    <t>264</t>
+  </si>
+  <si>
+    <t>265</t>
+  </si>
+  <si>
+    <t>266</t>
+  </si>
+  <si>
+    <t>267</t>
+  </si>
+  <si>
+    <t>268</t>
+  </si>
+  <si>
+    <t>269</t>
+  </si>
+  <si>
+    <t>270</t>
+  </si>
+  <si>
+    <t>271</t>
+  </si>
+  <si>
+    <t>272</t>
+  </si>
+  <si>
+    <t>273</t>
+  </si>
+  <si>
+    <t>274</t>
+  </si>
+  <si>
+    <t>275</t>
+  </si>
+  <si>
+    <t>276</t>
+  </si>
+  <si>
+    <t>277</t>
+  </si>
+  <si>
+    <t>278</t>
+  </si>
+  <si>
+    <t>279</t>
+  </si>
+  <si>
+    <t>280</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* &quot;-&quot;\ &quot;₽&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₽&quot;_-;\-* #,##0.00\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1525,15 +1656,19 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -1541,12 +1676,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="17"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="65"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1560,114 +1689,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0"/>
-    <cellStyle name="Percent" xfId="15"/>
-    <cellStyle name="Currency" xfId="16"/>
-    <cellStyle name="Currency [0]" xfId="17"/>
-    <cellStyle name="Comma" xfId="18"/>
-    <cellStyle name="Comma [0]" xfId="19"/>
+  <cellStyles count="7">
+    <cellStyle name="Comma" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Comma [0]" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Currency" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Currency [0]" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal" xfId="6" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Percent" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1990,14 +2043,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E241"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E281"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A240" workbookViewId="0">
+      <selection activeCell="J259" sqref="J259"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultColWidthPt="48.75" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="12.75">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2014,7 +2069,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="12.75">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2031,7 +2086,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="12.75">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2048,7 +2103,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="12.75">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -2065,7 +2120,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="12.75">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -2082,7 +2137,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="12.75">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2099,7 +2154,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="12.75">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -2116,7 +2171,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="12.75">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -2133,7 +2188,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="12.75">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -2150,7 +2205,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="12.75">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -2167,7 +2222,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="12.75">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -2184,7 +2239,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="12.75">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -2201,7 +2256,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="12.75">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -2218,7 +2273,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="12.75">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -2235,7 +2290,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="12.75">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -2252,7 +2307,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="12.75">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -2269,7 +2324,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="12.75">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -2286,7 +2341,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="12.75">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -2303,7 +2358,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="12.75">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>49</v>
       </c>
@@ -2320,7 +2375,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="12.75">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -2337,7 +2392,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="12.75">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>53</v>
       </c>
@@ -2354,7 +2409,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="12.75">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>55</v>
       </c>
@@ -2371,7 +2426,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="12.75">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>58</v>
       </c>
@@ -2388,7 +2443,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="12.75">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>60</v>
       </c>
@@ -2405,7 +2460,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="12.75">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>62</v>
       </c>
@@ -2422,7 +2477,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="12.75">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>64</v>
       </c>
@@ -2439,7 +2494,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="12.75">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>67</v>
       </c>
@@ -2456,7 +2511,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="12.75">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>69</v>
       </c>
@@ -2473,7 +2528,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="12.75">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>71</v>
       </c>
@@ -2490,7 +2545,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="12.75">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>73</v>
       </c>
@@ -2507,7 +2562,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="12.75">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>76</v>
       </c>
@@ -2524,7 +2579,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="12.75">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>78</v>
       </c>
@@ -2541,7 +2596,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="12.75">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>80</v>
       </c>
@@ -2558,7 +2613,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="12.75">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>82</v>
       </c>
@@ -2575,7 +2630,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="12.75">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>85</v>
       </c>
@@ -2592,7 +2647,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="12.75">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>87</v>
       </c>
@@ -2609,7 +2664,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="12.75">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>89</v>
       </c>
@@ -2626,7 +2681,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="12.75">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>91</v>
       </c>
@@ -2643,7 +2698,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="12.75">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>94</v>
       </c>
@@ -2660,7 +2715,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="12.75">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>96</v>
       </c>
@@ -2677,7 +2732,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="12.75">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>98</v>
       </c>
@@ -2694,7 +2749,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="12.75">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>100</v>
       </c>
@@ -2711,7 +2766,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="12.75">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>103</v>
       </c>
@@ -2728,7 +2783,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="12.75">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>105</v>
       </c>
@@ -2745,7 +2800,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="12.75">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>107</v>
       </c>
@@ -2762,7 +2817,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="12.75">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>109</v>
       </c>
@@ -2779,7 +2834,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="12.75">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>111</v>
       </c>
@@ -2796,7 +2851,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="12.75">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>113</v>
       </c>
@@ -2813,7 +2868,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="12.75">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>115</v>
       </c>
@@ -2830,7 +2885,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="12.75">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>117</v>
       </c>
@@ -2847,7 +2902,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="12.75">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>119</v>
       </c>
@@ -2864,7 +2919,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="12.75">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>121</v>
       </c>
@@ -2881,7 +2936,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="12.75">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>123</v>
       </c>
@@ -2898,7 +2953,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="12.75">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>125</v>
       </c>
@@ -2915,7 +2970,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="12.75">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>127</v>
       </c>
@@ -2932,7 +2987,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="12.75">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>129</v>
       </c>
@@ -2949,7 +3004,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="12.75">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>131</v>
       </c>
@@ -2966,7 +3021,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="12.75">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>133</v>
       </c>
@@ -2983,7 +3038,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="12.75">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>135</v>
       </c>
@@ -3000,7 +3055,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="12.75">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>137</v>
       </c>
@@ -3017,7 +3072,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="12.75">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>139</v>
       </c>
@@ -3034,7 +3089,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="12.75">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>141</v>
       </c>
@@ -3051,7 +3106,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="12.75">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>143</v>
       </c>
@@ -3068,7 +3123,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="12.75">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>145</v>
       </c>
@@ -3085,7 +3140,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="12.75">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>147</v>
       </c>
@@ -3102,7 +3157,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="12.75">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>149</v>
       </c>
@@ -3119,7 +3174,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="12.75">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>151</v>
       </c>
@@ -3136,7 +3191,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="12.75">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>153</v>
       </c>
@@ -3153,7 +3208,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="12.75">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>155</v>
       </c>
@@ -3170,7 +3225,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="12.75">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>157</v>
       </c>
@@ -3187,7 +3242,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="12.75">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>159</v>
       </c>
@@ -3204,7 +3259,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="12.75">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>161</v>
       </c>
@@ -3221,7 +3276,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="12.75">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>163</v>
       </c>
@@ -3238,7 +3293,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="12.75">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>165</v>
       </c>
@@ -3255,7 +3310,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="12.75">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>167</v>
       </c>
@@ -3272,7 +3327,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="12.75">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>169</v>
       </c>
@@ -3289,7 +3344,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="12.75">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>171</v>
       </c>
@@ -3306,7 +3361,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="12.75">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>173</v>
       </c>
@@ -3323,7 +3378,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="12.75">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>175</v>
       </c>
@@ -3340,7 +3395,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="12.75">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>177</v>
       </c>
@@ -3357,7 +3412,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="12.75">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>178</v>
       </c>
@@ -3374,7 +3429,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="12.75">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>180</v>
       </c>
@@ -3391,7 +3446,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="12.75">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>183</v>
       </c>
@@ -3408,7 +3463,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="12.75">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>185</v>
       </c>
@@ -3425,7 +3480,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="12.75">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>187</v>
       </c>
@@ -3442,7 +3497,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="12.75">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>189</v>
       </c>
@@ -3459,7 +3514,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="12.75">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>191</v>
       </c>
@@ -3476,7 +3531,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="12.75">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>193</v>
       </c>
@@ -3493,7 +3548,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="12.75">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>195</v>
       </c>
@@ -3510,7 +3565,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="12.75">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>197</v>
       </c>
@@ -3527,7 +3582,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="12.75">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>199</v>
       </c>
@@ -3544,7 +3599,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="12.75">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>201</v>
       </c>
@@ -3561,7 +3616,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="12.75">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>203</v>
       </c>
@@ -3578,7 +3633,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="12.75">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>205</v>
       </c>
@@ -3595,7 +3650,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="12.75">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>207</v>
       </c>
@@ -3612,7 +3667,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="12.75">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>209</v>
       </c>
@@ -3629,7 +3684,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="12.75">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>211</v>
       </c>
@@ -3646,7 +3701,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="12.75">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>213</v>
       </c>
@@ -3663,7 +3718,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="12.75">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>215</v>
       </c>
@@ -3680,7 +3735,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="12.75">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>217</v>
       </c>
@@ -3697,7 +3752,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="12.75">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>219</v>
       </c>
@@ -3714,7 +3769,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="12.75">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>221</v>
       </c>
@@ -3731,7 +3786,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="12.75">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>223</v>
       </c>
@@ -3748,7 +3803,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="12.75">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>225</v>
       </c>
@@ -3765,7 +3820,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="12.75">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>227</v>
       </c>
@@ -3782,7 +3837,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="12.75">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>229</v>
       </c>
@@ -3799,7 +3854,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="12.75">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>230</v>
       </c>
@@ -3816,7 +3871,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="12.75">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>232</v>
       </c>
@@ -3833,7 +3888,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="12.75">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>234</v>
       </c>
@@ -3850,7 +3905,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="12.75">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>236</v>
       </c>
@@ -3867,7 +3922,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="12.75">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>238</v>
       </c>
@@ -3884,7 +3939,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="12.75">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>240</v>
       </c>
@@ -3901,7 +3956,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="12.75">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>242</v>
       </c>
@@ -3918,7 +3973,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="12.75">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>244</v>
       </c>
@@ -3935,7 +3990,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="12.75">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>246</v>
       </c>
@@ -3952,7 +4007,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="12.75">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>248</v>
       </c>
@@ -3969,7 +4024,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="12.75">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>249</v>
       </c>
@@ -3986,7 +4041,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="12.75">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>251</v>
       </c>
@@ -4003,7 +4058,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="12.75">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>253</v>
       </c>
@@ -4020,7 +4075,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="12.75">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>255</v>
       </c>
@@ -4037,7 +4092,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="12.75">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>257</v>
       </c>
@@ -4054,7 +4109,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="12.75">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>259</v>
       </c>
@@ -4071,7 +4126,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="12.75">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>262</v>
       </c>
@@ -4088,7 +4143,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="12.75">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>264</v>
       </c>
@@ -4105,7 +4160,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="125" spans="1:5" ht="12.75">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>266</v>
       </c>
@@ -4122,7 +4177,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="126" spans="1:5" ht="12.75">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>268</v>
       </c>
@@ -4139,7 +4194,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="127" spans="1:5" ht="12.75">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>270</v>
       </c>
@@ -4156,7 +4211,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="128" spans="1:5" ht="12.75">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>272</v>
       </c>
@@ -4173,7 +4228,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="12.75">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>274</v>
       </c>
@@ -4190,7 +4245,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="12.75">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>276</v>
       </c>
@@ -4207,7 +4262,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="131" spans="1:5" ht="12.75">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>278</v>
       </c>
@@ -4224,7 +4279,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="12.75">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>280</v>
       </c>
@@ -4241,7 +4296,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="12.75">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>281</v>
       </c>
@@ -4258,7 +4313,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="12.75">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>283</v>
       </c>
@@ -4275,7 +4330,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="12.75">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>285</v>
       </c>
@@ -4292,7 +4347,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="12.75">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>287</v>
       </c>
@@ -4309,7 +4364,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="137" spans="1:5" ht="12.75">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>289</v>
       </c>
@@ -4326,7 +4381,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="138" spans="1:5" ht="12.75">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>291</v>
       </c>
@@ -4343,7 +4398,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="139" spans="1:5" ht="12.75">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>293</v>
       </c>
@@ -4360,7 +4415,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="12.75">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>295</v>
       </c>
@@ -4377,7 +4432,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="141" spans="1:5" ht="12.75">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>297</v>
       </c>
@@ -4394,7 +4449,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="142" spans="1:5" ht="12.75">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>299</v>
       </c>
@@ -4411,7 +4466,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="12.75">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>301</v>
       </c>
@@ -4428,7 +4483,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="12.75">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>303</v>
       </c>
@@ -4445,7 +4500,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="145" spans="1:5" ht="12.75">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>305</v>
       </c>
@@ -4462,7 +4517,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="146" spans="1:5" ht="12.75">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>307</v>
       </c>
@@ -4479,7 +4534,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="147" spans="1:5" ht="12.75">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>309</v>
       </c>
@@ -4496,7 +4551,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="148" spans="1:5" ht="12.75">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>311</v>
       </c>
@@ -4513,7 +4568,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="149" spans="1:5" ht="12.75">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>313</v>
       </c>
@@ -4530,7 +4585,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="150" spans="1:5" ht="12.75">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>315</v>
       </c>
@@ -4547,7 +4602,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="151" spans="1:5" ht="12.75">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>317</v>
       </c>
@@ -4564,7 +4619,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="152" spans="1:5" ht="12.75">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>319</v>
       </c>
@@ -4581,7 +4636,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="153" spans="1:5" ht="12.75">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>321</v>
       </c>
@@ -4598,7 +4653,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="154" spans="1:5" ht="12.75">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>323</v>
       </c>
@@ -4615,7 +4670,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="155" spans="1:5" ht="12.75">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>325</v>
       </c>
@@ -4632,7 +4687,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="156" spans="1:5" ht="12.75">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>327</v>
       </c>
@@ -4649,7 +4704,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="157" spans="1:5" ht="12.75">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>329</v>
       </c>
@@ -4666,7 +4721,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="158" spans="1:5" ht="12.75">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>331</v>
       </c>
@@ -4683,7 +4738,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="159" spans="1:5" ht="12.75">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>333</v>
       </c>
@@ -4700,7 +4755,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="160" spans="1:5" ht="12.75">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>335</v>
       </c>
@@ -4717,7 +4772,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="161" spans="1:5" ht="12.75">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>337</v>
       </c>
@@ -4734,7 +4789,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="162" spans="1:5" ht="12.75">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>339</v>
       </c>
@@ -4751,7 +4806,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="163" spans="1:5" ht="12.75">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>342</v>
       </c>
@@ -4768,7 +4823,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="164" spans="1:5" ht="12.75">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>344</v>
       </c>
@@ -4785,7 +4840,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="165" spans="1:5" ht="12.75">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>346</v>
       </c>
@@ -4802,7 +4857,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="166" spans="1:5" ht="12.75">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>348</v>
       </c>
@@ -4819,7 +4874,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="167" spans="1:5" ht="12.75">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>350</v>
       </c>
@@ -4836,7 +4891,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="168" spans="1:5" ht="12.75">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>352</v>
       </c>
@@ -4853,7 +4908,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="169" spans="1:5" ht="12.75">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>354</v>
       </c>
@@ -4870,7 +4925,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="170" spans="1:5" ht="12.75">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>356</v>
       </c>
@@ -4887,7 +4942,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="171" spans="1:5" ht="12.75">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>358</v>
       </c>
@@ -4904,7 +4959,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="172" spans="1:5" ht="12.75">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>360</v>
       </c>
@@ -4921,7 +4976,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="173" spans="1:5" ht="12.75">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>362</v>
       </c>
@@ -4938,7 +4993,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="174" spans="1:5" ht="12.75">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>364</v>
       </c>
@@ -4955,7 +5010,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="175" spans="1:5" ht="12.75">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>366</v>
       </c>
@@ -4972,7 +5027,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="176" spans="1:5" ht="12.75">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>368</v>
       </c>
@@ -4989,7 +5044,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="177" spans="1:5" ht="12.75">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>370</v>
       </c>
@@ -5006,7 +5061,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="178" spans="1:5" ht="12.75">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>372</v>
       </c>
@@ -5023,7 +5078,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="179" spans="1:5" ht="12.75">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>374</v>
       </c>
@@ -5040,7 +5095,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="180" spans="1:5" ht="12.75">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>375</v>
       </c>
@@ -5057,7 +5112,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="181" spans="1:5" ht="12.75">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>377</v>
       </c>
@@ -5074,7 +5129,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="182" spans="1:5" ht="12.75">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>379</v>
       </c>
@@ -5091,7 +5146,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="183" spans="1:5" ht="12.75">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>381</v>
       </c>
@@ -5108,7 +5163,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="184" spans="1:5" ht="12.75">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>383</v>
       </c>
@@ -5125,7 +5180,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="185" spans="1:5" ht="12.75">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>385</v>
       </c>
@@ -5142,7 +5197,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="186" spans="1:5" ht="12.75">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>387</v>
       </c>
@@ -5159,7 +5214,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="187" spans="1:5" ht="12.75">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>389</v>
       </c>
@@ -5176,7 +5231,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="188" spans="1:5" ht="12.75">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>391</v>
       </c>
@@ -5193,7 +5248,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="189" spans="1:5" ht="12.75">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>393</v>
       </c>
@@ -5210,7 +5265,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="190" spans="1:5" ht="12.75">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>395</v>
       </c>
@@ -5227,7 +5282,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="191" spans="1:5" ht="12.75">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>397</v>
       </c>
@@ -5244,7 +5299,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="192" spans="1:5" ht="12.75">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>399</v>
       </c>
@@ -5261,7 +5316,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="193" spans="1:5" ht="12.75">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>401</v>
       </c>
@@ -5278,7 +5333,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="194" spans="1:5" ht="12.75">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>403</v>
       </c>
@@ -5295,7 +5350,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="195" spans="1:5" ht="12.75">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>405</v>
       </c>
@@ -5312,7 +5367,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="196" spans="1:5" ht="12.75">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>407</v>
       </c>
@@ -5329,7 +5384,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="197" spans="1:5" ht="12.75">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>409</v>
       </c>
@@ -5346,7 +5401,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="198" spans="1:5" ht="12.75">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>411</v>
       </c>
@@ -5363,7 +5418,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="199" spans="1:5" ht="12.75">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>413</v>
       </c>
@@ -5380,7 +5435,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="200" spans="1:5" ht="12.75">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>415</v>
       </c>
@@ -5397,7 +5452,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="201" spans="1:5" ht="12.75">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>416</v>
       </c>
@@ -5414,7 +5469,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="202" spans="1:5" ht="12.75">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>418</v>
       </c>
@@ -5431,7 +5486,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="203" spans="1:5" ht="12.75">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>421</v>
       </c>
@@ -5448,7 +5503,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="204" spans="1:5" ht="12.75">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>423</v>
       </c>
@@ -5465,7 +5520,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="205" spans="1:5" ht="12.75">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>425</v>
       </c>
@@ -5482,7 +5537,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="206" spans="1:5" ht="12.75">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>427</v>
       </c>
@@ -5499,7 +5554,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="207" spans="1:5" ht="12.75">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>429</v>
       </c>
@@ -5516,7 +5571,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="208" spans="1:5" ht="12.75">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>431</v>
       </c>
@@ -5533,7 +5588,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="209" spans="1:5" ht="12.75">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>433</v>
       </c>
@@ -5550,7 +5605,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="210" spans="1:5" ht="12.75">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>435</v>
       </c>
@@ -5567,7 +5622,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="211" spans="1:5" ht="12.75">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>437</v>
       </c>
@@ -5584,7 +5639,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="212" spans="1:5" ht="12.75">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>439</v>
       </c>
@@ -5601,7 +5656,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="213" spans="1:5" ht="12.75">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>441</v>
       </c>
@@ -5618,7 +5673,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="214" spans="1:5" ht="12.75">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>443</v>
       </c>
@@ -5635,7 +5690,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="215" spans="1:5" ht="12.75">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>444</v>
       </c>
@@ -5652,7 +5707,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="216" spans="1:5" ht="12.75">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>446</v>
       </c>
@@ -5669,7 +5724,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="217" spans="1:5" ht="12.75">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>448</v>
       </c>
@@ -5686,7 +5741,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="218" spans="1:5" ht="12.75">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>450</v>
       </c>
@@ -5703,7 +5758,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="219" spans="1:5" ht="12.75">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>452</v>
       </c>
@@ -5720,7 +5775,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="220" spans="1:5" ht="12.75">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>454</v>
       </c>
@@ -5737,7 +5792,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="221" spans="1:5" ht="12.75">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>455</v>
       </c>
@@ -5754,7 +5809,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="222" spans="1:5" ht="12.75">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>457</v>
       </c>
@@ -5771,7 +5826,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="223" spans="1:5" ht="12.75">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>459</v>
       </c>
@@ -5788,7 +5843,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="224" spans="1:5" ht="12.75">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>461</v>
       </c>
@@ -5805,7 +5860,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="225" spans="1:5" ht="12.75">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>463</v>
       </c>
@@ -5822,7 +5877,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="226" spans="1:5" ht="12.75">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>465</v>
       </c>
@@ -5839,7 +5894,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="227" spans="1:5" ht="12.75">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>467</v>
       </c>
@@ -5856,7 +5911,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="228" spans="1:5" ht="12.75">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>469</v>
       </c>
@@ -5873,7 +5928,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="229" spans="1:5" ht="12.75">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>471</v>
       </c>
@@ -5890,7 +5945,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="230" spans="1:5" ht="12.75">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>473</v>
       </c>
@@ -5907,7 +5962,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="231" spans="1:5" ht="12.75">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>474</v>
       </c>
@@ -5924,7 +5979,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="232" spans="1:5" ht="12.75">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>476</v>
       </c>
@@ -5941,7 +5996,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="233" spans="1:5" ht="12.75">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>478</v>
       </c>
@@ -5958,7 +6013,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="234" spans="1:5" ht="12.75">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>480</v>
       </c>
@@ -5975,7 +6030,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="235" spans="1:5" ht="12.75">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>482</v>
       </c>
@@ -5992,7 +6047,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="236" spans="1:5" ht="12.75">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>484</v>
       </c>
@@ -6009,7 +6064,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="237" spans="1:5" ht="12.75">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>486</v>
       </c>
@@ -6026,7 +6081,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="238" spans="1:5" ht="12.75">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>488</v>
       </c>
@@ -6043,7 +6098,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="239" spans="1:5" ht="12.75">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>490</v>
       </c>
@@ -6060,7 +6115,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="240" spans="1:5" ht="12.75">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>492</v>
       </c>
@@ -6077,7 +6132,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="241" spans="1:5" ht="12.75">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>494</v>
       </c>
@@ -6094,37 +6149,595 @@
         <v>495</v>
       </c>
     </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A242" t="s">
+        <v>496</v>
+      </c>
+      <c r="B242">
+        <v>2024</v>
+      </c>
+      <c r="C242" t="s">
+        <v>7</v>
+      </c>
+      <c r="D242" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A243" t="s">
+        <v>497</v>
+      </c>
+      <c r="B243">
+        <v>2024</v>
+      </c>
+      <c r="C243" t="s">
+        <v>7</v>
+      </c>
+      <c r="D243" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A244" t="s">
+        <v>498</v>
+      </c>
+      <c r="B244">
+        <v>2024</v>
+      </c>
+      <c r="C244" t="s">
+        <v>7</v>
+      </c>
+      <c r="D244" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A245" t="s">
+        <v>499</v>
+      </c>
+      <c r="B245">
+        <v>2024</v>
+      </c>
+      <c r="C245" t="s">
+        <v>7</v>
+      </c>
+      <c r="D245" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A246" t="s">
+        <v>500</v>
+      </c>
+      <c r="B246">
+        <v>2024</v>
+      </c>
+      <c r="C246" t="s">
+        <v>20</v>
+      </c>
+      <c r="D246" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A247" t="s">
+        <v>501</v>
+      </c>
+      <c r="B247">
+        <v>2024</v>
+      </c>
+      <c r="C247" t="s">
+        <v>20</v>
+      </c>
+      <c r="D247" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A248" t="s">
+        <v>502</v>
+      </c>
+      <c r="B248">
+        <v>2024</v>
+      </c>
+      <c r="C248" t="s">
+        <v>20</v>
+      </c>
+      <c r="D248" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A249" t="s">
+        <v>503</v>
+      </c>
+      <c r="B249">
+        <v>2024</v>
+      </c>
+      <c r="C249" t="s">
+        <v>20</v>
+      </c>
+      <c r="D249" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A250" t="s">
+        <v>504</v>
+      </c>
+      <c r="B250">
+        <v>2024</v>
+      </c>
+      <c r="C250" t="s">
+        <v>29</v>
+      </c>
+      <c r="D250" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A251" t="s">
+        <v>505</v>
+      </c>
+      <c r="B251">
+        <v>2024</v>
+      </c>
+      <c r="C251" t="s">
+        <v>29</v>
+      </c>
+      <c r="D251" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A252" t="s">
+        <v>506</v>
+      </c>
+      <c r="B252">
+        <v>2024</v>
+      </c>
+      <c r="C252" t="s">
+        <v>29</v>
+      </c>
+      <c r="D252" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A253" t="s">
+        <v>507</v>
+      </c>
+      <c r="B253">
+        <v>2024</v>
+      </c>
+      <c r="C253" t="s">
+        <v>29</v>
+      </c>
+      <c r="D253" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A254" t="s">
+        <v>508</v>
+      </c>
+      <c r="B254">
+        <v>2024</v>
+      </c>
+      <c r="C254" t="s">
+        <v>38</v>
+      </c>
+      <c r="D254" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A255" t="s">
+        <v>509</v>
+      </c>
+      <c r="B255">
+        <v>2024</v>
+      </c>
+      <c r="C255" t="s">
+        <v>38</v>
+      </c>
+      <c r="D255" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A256" t="s">
+        <v>510</v>
+      </c>
+      <c r="B256">
+        <v>2024</v>
+      </c>
+      <c r="C256" t="s">
+        <v>38</v>
+      </c>
+      <c r="D256" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A257" t="s">
+        <v>511</v>
+      </c>
+      <c r="B257">
+        <v>2024</v>
+      </c>
+      <c r="C257" t="s">
+        <v>38</v>
+      </c>
+      <c r="D257" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A258" t="s">
+        <v>512</v>
+      </c>
+      <c r="B258">
+        <v>2024</v>
+      </c>
+      <c r="C258" t="s">
+        <v>47</v>
+      </c>
+      <c r="D258" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A259" t="s">
+        <v>513</v>
+      </c>
+      <c r="B259">
+        <v>2024</v>
+      </c>
+      <c r="C259" t="s">
+        <v>47</v>
+      </c>
+      <c r="D259" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A260" t="s">
+        <v>514</v>
+      </c>
+      <c r="B260">
+        <v>2024</v>
+      </c>
+      <c r="C260" t="s">
+        <v>47</v>
+      </c>
+      <c r="D260" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A261" t="s">
+        <v>515</v>
+      </c>
+      <c r="B261">
+        <v>2024</v>
+      </c>
+      <c r="C261" t="s">
+        <v>47</v>
+      </c>
+      <c r="D261" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A262" t="s">
+        <v>516</v>
+      </c>
+      <c r="B262">
+        <v>2024</v>
+      </c>
+      <c r="C262" t="s">
+        <v>56</v>
+      </c>
+      <c r="D262" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A263" t="s">
+        <v>517</v>
+      </c>
+      <c r="B263">
+        <v>2024</v>
+      </c>
+      <c r="C263" t="s">
+        <v>56</v>
+      </c>
+      <c r="D263" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A264" t="s">
+        <v>518</v>
+      </c>
+      <c r="B264">
+        <v>2024</v>
+      </c>
+      <c r="C264" t="s">
+        <v>56</v>
+      </c>
+      <c r="D264" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A265" t="s">
+        <v>519</v>
+      </c>
+      <c r="B265">
+        <v>2024</v>
+      </c>
+      <c r="C265" t="s">
+        <v>56</v>
+      </c>
+      <c r="D265" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A266" t="s">
+        <v>520</v>
+      </c>
+      <c r="B266">
+        <v>2024</v>
+      </c>
+      <c r="C266" t="s">
+        <v>65</v>
+      </c>
+      <c r="D266" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A267" t="s">
+        <v>521</v>
+      </c>
+      <c r="B267">
+        <v>2024</v>
+      </c>
+      <c r="C267" t="s">
+        <v>65</v>
+      </c>
+      <c r="D267" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A268" t="s">
+        <v>522</v>
+      </c>
+      <c r="B268">
+        <v>2024</v>
+      </c>
+      <c r="C268" t="s">
+        <v>65</v>
+      </c>
+      <c r="D268" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A269" t="s">
+        <v>523</v>
+      </c>
+      <c r="B269">
+        <v>2024</v>
+      </c>
+      <c r="C269" t="s">
+        <v>65</v>
+      </c>
+      <c r="D269" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A270" t="s">
+        <v>524</v>
+      </c>
+      <c r="B270">
+        <v>2024</v>
+      </c>
+      <c r="C270" t="s">
+        <v>74</v>
+      </c>
+      <c r="D270" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A271" t="s">
+        <v>525</v>
+      </c>
+      <c r="B271">
+        <v>2024</v>
+      </c>
+      <c r="C271" t="s">
+        <v>74</v>
+      </c>
+      <c r="D271" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A272" t="s">
+        <v>526</v>
+      </c>
+      <c r="B272">
+        <v>2024</v>
+      </c>
+      <c r="C272" t="s">
+        <v>74</v>
+      </c>
+      <c r="D272" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A273" t="s">
+        <v>527</v>
+      </c>
+      <c r="B273">
+        <v>2024</v>
+      </c>
+      <c r="C273" t="s">
+        <v>74</v>
+      </c>
+      <c r="D273" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A274" t="s">
+        <v>528</v>
+      </c>
+      <c r="B274">
+        <v>2024</v>
+      </c>
+      <c r="C274" t="s">
+        <v>83</v>
+      </c>
+      <c r="D274" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A275" t="s">
+        <v>529</v>
+      </c>
+      <c r="B275">
+        <v>2024</v>
+      </c>
+      <c r="C275" t="s">
+        <v>83</v>
+      </c>
+      <c r="D275" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A276" t="s">
+        <v>530</v>
+      </c>
+      <c r="B276">
+        <v>2024</v>
+      </c>
+      <c r="C276" t="s">
+        <v>83</v>
+      </c>
+      <c r="D276" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A277" t="s">
+        <v>531</v>
+      </c>
+      <c r="B277">
+        <v>2024</v>
+      </c>
+      <c r="C277" t="s">
+        <v>83</v>
+      </c>
+      <c r="D277" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A278" t="s">
+        <v>532</v>
+      </c>
+      <c r="B278">
+        <v>2024</v>
+      </c>
+      <c r="C278" t="s">
+        <v>92</v>
+      </c>
+      <c r="D278" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A279" t="s">
+        <v>533</v>
+      </c>
+      <c r="B279">
+        <v>2024</v>
+      </c>
+      <c r="C279" t="s">
+        <v>92</v>
+      </c>
+      <c r="D279" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A280" t="s">
+        <v>534</v>
+      </c>
+      <c r="B280">
+        <v>2024</v>
+      </c>
+      <c r="C280" t="s">
+        <v>92</v>
+      </c>
+      <c r="D280" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A281" t="s">
+        <v>535</v>
+      </c>
+      <c r="B281">
+        <v>2024</v>
+      </c>
+      <c r="C281" t="s">
+        <v>92</v>
+      </c>
+      <c r="D281" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultColWidthPt="48.75" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
-  <printOptions/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultColWidthPt="48.75" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
-  <printOptions/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>